<commit_message>
NEW projects list updated
</commit_message>
<xml_diff>
--- a/data/projects.xlsx
+++ b/data/projects.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t xml:space="preserve">status</t>
   </si>
@@ -70,7 +70,25 @@
     <t xml:space="preserve">The webapp manages reservations, dynamic menu and social sharing APIs.</t>
   </si>
   <si>
-    <t xml:space="preserve">quotations.opinioni.net</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://quotations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.opinioni.net</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Gestione preventivi e progetti</t>
@@ -80,6 +98,42 @@
   </si>
   <si>
     <t xml:space="preserve">L’applicazione permette di gestire comodamente I preventivi ed I lavori/progetti fatti nel corso del tempo. Svluppato per Demetra Opinioni.net srl.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The webapp allows you to manage quotations and projects for customers and employees.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bpi.demetra.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panel online per pmi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panel online for businesses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sviluppato con il team IT di Demetra Opinioni.net, BPI è un panel per imprese, in cui un manager o un responsabile di un qualsiasi business può registrare la propria azienda e rispondere a questionari in cambio di premi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panel BPI is an online Panel for medium/small businesses. Any manager of any business can subscribe its business and will receive some prizes after answering surveys. Developed with the IT team of Demetra Opinioni.net.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://kirpachov.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sito web personale di Oleksandr Kirpachov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oleksandr Kirpachov’s personal website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il mio sito personale è utile a trovare nuovi clienti e fornire un comodo contatto ai clienti esistenti.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This website is useful to find new customers, and let the old customers a place where they can reach me out.</t>
   </si>
 </sst>
 </file>
@@ -90,11 +144,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -110,6 +165,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -154,7 +216,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -164,6 +226,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -187,12 +253,12 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="38.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="117.72"/>
@@ -266,7 +332,7 @@
       <c r="C3" s="1" t="n">
         <v>44986</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -281,12 +347,64 @@
       <c r="H3" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="I3" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E4" s="2"/>
+      <c r="A4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>44682</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>44927</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E5" s="2"/>
+      <c r="A5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>44986</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E6" s="2"/>
@@ -298,6 +416,10 @@
       <c r="E8" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" display="https://quotations"/>
+    <hyperlink ref="D5" r:id="rId2" display="https://kirpachov.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>